<commit_message>
Updates to electricity exponent and shareweights
</commit_message>
<xml_diff>
--- a/InputData/elec/ETLE/Electricity Technology Logit Exponent.xlsx
+++ b/InputData/elec/ETLE/Electricity Technology Logit Exponent.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeRepositories\eps-us\InputData\elec\ETLE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\elec\ETLE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DAD0BFF-2786-4443-AD14-A32093EDDD8A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{656C0D64-7DBC-460F-B7A8-761BCC4B2C11}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24810" yWindow="3630" windowWidth="28560" windowHeight="19110" xr2:uid="{9B08635C-C98A-4192-B8F2-5981CE9EC6E6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{9B08635C-C98A-4192-B8F2-5981CE9EC6E6}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="ETLE" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -520,7 +520,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -541,7 +543,7 @@
         <v>12</v>
       </c>
       <c r="B2">
-        <v>-3</v>
+        <v>-5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix some pre-run and runtime errors (#232)
</commit_message>
<xml_diff>
--- a/InputData/elec/ETLE/Electricity Technology Logit Exponent.xlsx
+++ b/InputData/elec/ETLE/Electricity Technology Logit Exponent.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\elec\ETLE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff Rissman\CodeRepositories\eps-us\InputData\elec\ETLE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{656C0D64-7DBC-460F-B7A8-761BCC4B2C11}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{375E25B1-CED6-4BC4-A116-A5CAE03023A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{9B08635C-C98A-4192-B8F2-5981CE9EC6E6}"/>
+    <workbookView xWindow="19140" yWindow="3480" windowWidth="34740" windowHeight="19920" xr2:uid="{9B08635C-C98A-4192-B8F2-5981CE9EC6E6}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -520,9 +520,7 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -543,7 +541,7 @@
         <v>12</v>
       </c>
       <c r="B2">
-        <v>-5</v>
+        <v>-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improvements to reliability-based construction and first attempt to implement capacity market payments (#232)
</commit_message>
<xml_diff>
--- a/InputData/elec/ETLE/Electricity Technology Logit Exponent.xlsx
+++ b/InputData/elec/ETLE/Electricity Technology Logit Exponent.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff Rissman\CodeRepositories\eps-us\InputData\elec\ETLE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{521EB69E-B8F6-4D94-BBFE-6709CE56E7C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45FE6818-3D06-410E-A8EE-0D0110330692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11280" yWindow="1020" windowWidth="34740" windowHeight="19920" xr2:uid="{9B08635C-C98A-4192-B8F2-5981CE9EC6E6}"/>
+    <workbookView xWindow="25515" yWindow="210" windowWidth="31110" windowHeight="20640" xr2:uid="{9B08635C-C98A-4192-B8F2-5981CE9EC6E6}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>Exponent</t>
   </si>
@@ -78,21 +78,6 @@
   </si>
   <si>
     <t>ETLE Electricity Technology Logit Exponents</t>
-  </si>
-  <si>
-    <t>The larger the numerical quantity being allocated, the more negative an exponent can be</t>
-  </si>
-  <si>
-    <t>tolerated.  If the exponent is too negative for the quantities being allocated, they will</t>
-  </si>
-  <si>
-    <t>get rounded to zero, and nothing will be allocated.  This is why there are two versions</t>
-  </si>
-  <si>
-    <t>of ETLE - one for allocating output (in MWh) and one for allocating capacity (in MW).</t>
-  </si>
-  <si>
-    <t>Output in MW has much larger numbers and tolerates a more negative ETLE value.</t>
   </si>
 </sst>
 </file>
@@ -465,7 +450,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6422D012-50FD-4D0C-A3BE-19778A6AC198}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -516,36 +501,11 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
         <v>10</v>
       </c>
     </row>
@@ -619,7 +579,7 @@
         <v>11</v>
       </c>
       <c r="B2">
-        <v>-1</v>
+        <v>-5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to Annual Capex correcting data issues. Updates to fraction of start year cpacity retire per unit net loss, calibrated (uses latest fuel price data). Updates to ETLE-capacity to move to -8.
</commit_message>
<xml_diff>
--- a/InputData/elec/ETLE/Electricity Technology Logit Exponent.xlsx
+++ b/InputData/elec/ETLE/Electricity Technology Logit Exponent.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff Rissman\CodeRepositories\eps-us\InputData\elec\ETLE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\elec\ETLE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45FE6818-3D06-410E-A8EE-0D0110330692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E8B89F9-6804-470F-B4EA-4B6C61AEF9DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25515" yWindow="210" windowWidth="31110" windowHeight="20640" xr2:uid="{9B08635C-C98A-4192-B8F2-5981CE9EC6E6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" xr2:uid="{9B08635C-C98A-4192-B8F2-5981CE9EC6E6}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -558,7 +558,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -579,7 +581,7 @@
         <v>11</v>
       </c>
       <c r="B2">
-        <v>-5</v>
+        <v>-8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implements unmodified logit for reliability based capacity expansion; addresses missing energy market revenue estimates for plants with no start year capacity; updates capacity factors for CCS power plants to align with non-CCS counterparts; changes boolean for whether or not certain plants bid at expected or peak capacity factors.
</commit_message>
<xml_diff>
--- a/InputData/elec/ETLE/Electricity Technology Logit Exponent.xlsx
+++ b/InputData/elec/ETLE/Electricity Technology Logit Exponent.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\elec\ETLE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E8B89F9-6804-470F-B4EA-4B6C61AEF9DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE33E77B-0D26-415E-BCA3-EC864F2A6336}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" xr2:uid="{9B08635C-C98A-4192-B8F2-5981CE9EC6E6}"/>
+    <workbookView xWindow="1350" yWindow="1905" windowWidth="32595" windowHeight="21495" activeTab="2" xr2:uid="{9B08635C-C98A-4192-B8F2-5981CE9EC6E6}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -452,7 +452,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6422D012-50FD-4D0C-A3BE-19778A6AC198}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -558,7 +558,7 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -581,7 +581,7 @@
         <v>11</v>
       </c>
       <c r="B2">
-        <v>-8</v>
+        <v>-0.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adds tiered cost system in for reliability based additions, cleans up codes, two calibrated data updates.
</commit_message>
<xml_diff>
--- a/InputData/elec/ETLE/Electricity Technology Logit Exponent.xlsx
+++ b/InputData/elec/ETLE/Electricity Technology Logit Exponent.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\elec\ETLE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE33E77B-0D26-415E-BCA3-EC864F2A6336}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4C7030B-C51E-4BFD-BC7C-7D7F47372D38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1350" yWindow="1905" windowWidth="32595" windowHeight="21495" activeTab="2" xr2:uid="{9B08635C-C98A-4192-B8F2-5981CE9EC6E6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="2" xr2:uid="{9B08635C-C98A-4192-B8F2-5981CE9EC6E6}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -559,7 +559,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,7 +581,7 @@
         <v>11</v>
       </c>
       <c r="B2">
-        <v>-0.3</v>
+        <v>-90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>